<commit_message>
Swapped 3 functions for new ones, generated plots & calculated values
</commit_message>
<xml_diff>
--- a/10D_values.xlsx
+++ b/10D_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milanjanovic/Documents/GitHub/AK9EV_Zapocet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{525755A4-DCA0-C540-8A35-4BA029171FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B26160-8ACD-DF48-A050-EC81DFB36B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16700" xr2:uid="{60C445AB-C4BF-6A4F-8E0D-E873C8E3AA26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>3.981494375953014e-07</t>
   </si>
@@ -197,12 +197,6 @@
     <t>-0.9999956670407897</t>
   </si>
   <si>
-    <t>0.9668481852717419</t>
-  </si>
-  <si>
-    <t>0.9999997371270192</t>
-  </si>
-  <si>
     <t>1.0000000000004474</t>
   </si>
   <si>
@@ -275,21 +269,6 @@
     <t>0.2975224610767144</t>
   </si>
   <si>
-    <t>1.5092987573193726e-19</t>
-  </si>
-  <si>
-    <t>14480.385551182912</t>
-  </si>
-  <si>
-    <t>5.3732718781188296e-64</t>
-  </si>
-  <si>
-    <t>1.6794829548601302e-189</t>
-  </si>
-  <si>
-    <t>10.08947473264175</t>
-  </si>
-  <si>
     <t>1.0000004629936439</t>
   </si>
   <si>
@@ -317,21 +296,6 @@
     <t>-0.06450680892731832</t>
   </si>
   <si>
-    <t>3.0225925958508326e-07</t>
-  </si>
-  <si>
-    <t>2.8298919506774</t>
-  </si>
-  <si>
-    <t>2.0724163126336253e-16</t>
-  </si>
-  <si>
-    <t>1.0384286023660522e-14</t>
-  </si>
-  <si>
-    <t>0.23348372918231508</t>
-  </si>
-  <si>
     <t>-5.759620019472256</t>
   </si>
   <si>
@@ -357,6 +321,51 @@
   </si>
   <si>
     <t>-0.9999999999333162</t>
+  </si>
+  <si>
+    <t>9.949606901118928</t>
+  </si>
+  <si>
+    <t>4232.344860355826</t>
+  </si>
+  <si>
+    <t>23.87899386041662</t>
+  </si>
+  <si>
+    <t>1712.8018786815285</t>
+  </si>
+  <si>
+    <t>193.00944824678695</t>
+  </si>
+  <si>
+    <t>20.19548284026875</t>
+  </si>
+  <si>
+    <t>19.707291487390858</t>
+  </si>
+  <si>
+    <t>12.793175074039507</t>
+  </si>
+  <si>
+    <t>17.90139807074293</t>
+  </si>
+  <si>
+    <t>15.936904983294832</t>
+  </si>
+  <si>
+    <t>-6.833489694206217</t>
+  </si>
+  <si>
+    <t>-7.410010461409956</t>
+  </si>
+  <si>
+    <t>-6.922172446724602</t>
+  </si>
+  <si>
+    <t>-5.387904107804386</t>
+  </si>
+  <si>
+    <t>-5.74372895841017</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,7 +727,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E25" sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,206 +962,206 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Values sheets adjustments for new fucntions
</commit_message>
<xml_diff>
--- a/10D_values.xlsx
+++ b/10D_values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milanjanovic/Documents/GitHub/AK9EV_Zapocet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B26160-8ACD-DF48-A050-EC81DFB36B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF2339-A4F2-1A45-8E94-0B1F18123357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16700" xr2:uid="{60C445AB-C4BF-6A4F-8E0D-E873C8E3AA26}"/>
   </bookViews>
@@ -36,110 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
-  <si>
-    <t>3.981494375953014e-07</t>
-  </si>
-  <si>
-    <t>19.910200939332398</t>
-  </si>
-  <si>
-    <t>9.419457966439465e-22</t>
-  </si>
-  <si>
-    <t>4.860241421116346e-63</t>
-  </si>
-  <si>
-    <t>1.1584488013581349</t>
-  </si>
-  <si>
-    <t>8.057393734268216e-07</t>
-  </si>
-  <si>
-    <t>36.560032348227224</t>
-  </si>
-  <si>
-    <t>1.2522284450528465e-21</t>
-  </si>
-  <si>
-    <t>1.8057764888840616e-63</t>
-  </si>
-  <si>
-    <t>1.5598804749425192</t>
-  </si>
-  <si>
-    <t>4.773860133424509e-13</t>
-  </si>
-  <si>
-    <t>512.9941234843735</t>
-  </si>
-  <si>
-    <t>5.495669494771366e-42</t>
-  </si>
-  <si>
-    <t>6.127369839998088e-127</t>
-  </si>
-  <si>
-    <t>1.9987328319810809</t>
-  </si>
-  <si>
-    <t>-0.9999999684947506</t>
-  </si>
-  <si>
-    <t>-0.9999986526411705</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t>-1.0</t>
   </si>
   <si>
-    <t>-0.9999999963536037</t>
-  </si>
-  <si>
-    <t>-0.9999999999561712</t>
-  </si>
-  <si>
-    <t>-0.9999999695119592</t>
-  </si>
-  <si>
-    <t>-0.9999981707197296</t>
-  </si>
-  <si>
-    <t>-0.9999999948681029</t>
-  </si>
-  <si>
-    <t>-0.9999999999454702</t>
-  </si>
-  <si>
-    <t>1.0000003742946582</t>
-  </si>
-  <si>
-    <t>5489508781.324987</t>
-  </si>
-  <si>
     <t>1.0000000000000002</t>
   </si>
   <si>
-    <t>1.000000000000025</t>
-  </si>
-  <si>
-    <t>3.19813463897961</t>
-  </si>
-  <si>
-    <t>6.396715701912272e-96</t>
-  </si>
-  <si>
-    <t>1.2836281682930826e-89</t>
-  </si>
-  <si>
-    <t>3.4040717702408437e-87</t>
-  </si>
-  <si>
-    <t>6.396714493032401e-96</t>
-  </si>
-  <si>
-    <t>1.9316647926767462e-95</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
@@ -197,33 +101,6 @@
     <t>-0.9999956670407897</t>
   </si>
   <si>
-    <t>1.0000000000004474</t>
-  </si>
-  <si>
-    <t>536.8845074508746</t>
-  </si>
-  <si>
-    <t>1.0000000000000036</t>
-  </si>
-  <si>
-    <t>2.096530449350951</t>
-  </si>
-  <si>
-    <t>-99998.99984343992</t>
-  </si>
-  <si>
-    <t>-90813.04370465297</t>
-  </si>
-  <si>
-    <t>-94819.508357029</t>
-  </si>
-  <si>
-    <t>-99998.99999999975</t>
-  </si>
-  <si>
-    <t>-99535.73452566713</t>
-  </si>
-  <si>
     <t>0.0006850715577982568</t>
   </si>
   <si>
@@ -366,6 +243,156 @@
   </si>
   <si>
     <t>-5.74372895841017</t>
+  </si>
+  <si>
+    <t>0.020142591449572332</t>
+  </si>
+  <si>
+    <t>35.85710300355927</t>
+  </si>
+  <si>
+    <t>0.05614235344305322</t>
+  </si>
+  <si>
+    <t>46.89086545329791</t>
+  </si>
+  <si>
+    <t>12.550227652111586</t>
+  </si>
+  <si>
+    <t>0.25163275703033333</t>
+  </si>
+  <si>
+    <t>0.4923015509874489</t>
+  </si>
+  <si>
+    <t>0.08852651295347967</t>
+  </si>
+  <si>
+    <t>0.4837727168770844</t>
+  </si>
+  <si>
+    <t>0.35505778315925246</t>
+  </si>
+  <si>
+    <t>0.015144134188150575</t>
+  </si>
+  <si>
+    <t>110.01527412398696</t>
+  </si>
+  <si>
+    <t>0.1452486202246296</t>
+  </si>
+  <si>
+    <t>239.5643584022369</t>
+  </si>
+  <si>
+    <t>10.19914992975199</t>
+  </si>
+  <si>
+    <t>-1387.6698389089258</t>
+  </si>
+  <si>
+    <t>-695.0922489817822</t>
+  </si>
+  <si>
+    <t>-701.8285753379513</t>
+  </si>
+  <si>
+    <t>-756.3098928132179</t>
+  </si>
+  <si>
+    <t>-648.0688983811172</t>
+  </si>
+  <si>
+    <t>0.7087745513083609</t>
+  </si>
+  <si>
+    <t>10684909.820605008</t>
+  </si>
+  <si>
+    <t>15.294301320987415</t>
+  </si>
+  <si>
+    <t>0.7973158224694807</t>
+  </si>
+  <si>
+    <t>16717.415508524267</t>
+  </si>
+  <si>
+    <t>1.0989938374288007e-06</t>
+  </si>
+  <si>
+    <t>4707.664953204047</t>
+  </si>
+  <si>
+    <t>3.565465430051976e-15</t>
+  </si>
+  <si>
+    <t>7.091693651262231e-94</t>
+  </si>
+  <si>
+    <t>576.8561949029591</t>
+  </si>
+  <si>
+    <t>0.12307553363847566</t>
+  </si>
+  <si>
+    <t>1.8332066791801442</t>
+  </si>
+  <si>
+    <t>0.18320667918015018</t>
+  </si>
+  <si>
+    <t>3.187212264075637</t>
+  </si>
+  <si>
+    <t>0.7505564472414155</t>
+  </si>
+  <si>
+    <t>1.3158351035989628</t>
+  </si>
+  <si>
+    <t>2.461963219952342</t>
+  </si>
+  <si>
+    <t>1.4910517842354136</t>
+  </si>
+  <si>
+    <t>2.447271144489616</t>
+  </si>
+  <si>
+    <t>1.9305259714704959</t>
+  </si>
+  <si>
+    <t>3553.4791804844563</t>
+  </si>
+  <si>
+    <t>3692.458764845495</t>
+  </si>
+  <si>
+    <t>3724.5883078363386</t>
+  </si>
+  <si>
+    <t>3642.050187847467</t>
+  </si>
+  <si>
+    <t>3733.051694310899</t>
+  </si>
+  <si>
+    <t>0.6666666758676818</t>
+  </si>
+  <si>
+    <t>2727651.1036712644</t>
+  </si>
+  <si>
+    <t>0.6222222221202239</t>
+  </si>
+  <si>
+    <t>0.44444444406686484</t>
+  </si>
+  <si>
+    <t>5654.924639682926</t>
   </si>
 </sst>
 </file>
@@ -727,7 +754,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="A1:E25"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,427 +768,427 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>